<commit_message>
Updated and finished implementing the terraforming section of the tutorial.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{201808C7-738F-4A5B-B823-BFA6AE351049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B6A94A65-08A7-4570-A1E9-725F90C68511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue, v2.xlsx" sheetId="1" r:id="rId1"/>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>Terraforming</t>
-  </si>
-  <si>
-    <t>got power and water</t>
   </si>
   <si>
     <t>Wonderful! Now let's look at the buildings that will contribute progress to the terraforming tower.</t>
@@ -562,9 +559,6 @@
     <t>Stored in my memory are blueprints of buildings that can be used to make this barren planet a paradise for your humans.</t>
   </si>
   <si>
-    <t>Next,  build an /ice drill\! Look for a blue patch.</t>
-  </si>
-  <si>
     <t>First, you'll need power. Please build a [fusion reactor].</t>
   </si>
   <si>
@@ -581,6 +575,12 @@
   </si>
   <si>
     <t>Construction system: online.~External environment scanner: online.~Construction system: enabled.~All systems are online.~Task: terraform this planet for human habitation. Begin.</t>
+  </si>
+  <si>
+    <t>got resources</t>
+  </si>
+  <si>
+    <t>Try building an /ice drill\! Look for a blue patch.</t>
   </si>
 </sst>
 </file>
@@ -1361,8 +1361,8 @@
   <dimension ref="A1:XFD993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1397,16 +1397,16 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="12.75">
       <c r="A2" s="56" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="27"/>
@@ -1472,13 +1472,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
@@ -1488,13 +1488,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -1520,13 +1520,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="30"/>
@@ -1542,7 +1542,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27" t="s">
@@ -1578,7 +1578,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
@@ -1594,7 +1594,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -1610,7 +1610,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
@@ -1626,7 +1626,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1642,7 +1642,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="31"/>
@@ -1676,7 +1676,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="27" t="s">
@@ -1694,7 +1694,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
@@ -1710,7 +1710,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="36" t="s">
@@ -1750,7 +1750,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>36</v>
@@ -1770,7 +1770,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="41" t="s">
@@ -1804,7 +1804,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27" t="s">
@@ -1844,7 +1844,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36" t="s">
@@ -1884,7 +1884,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="71" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>47</v>
@@ -1904,7 +1904,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -1922,7 +1922,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
@@ -1938,7 +1938,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="36" t="s">
@@ -1978,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>53</v>
@@ -1998,7 +1998,7 @@
         <v>55</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="36" t="s">
@@ -2016,7 +2016,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>57</v>
@@ -2033,14 +2033,14 @@
         <v>25</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>60</v>
+        <v>184</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="12.75">
@@ -2051,10 +2051,10 @@
         <v>7</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="36" t="s">
@@ -2091,14 +2091,14 @@
         <v>25</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="12.75">
@@ -2109,14 +2109,14 @@
         <v>25</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:28" ht="12.75">
@@ -2127,14 +2127,14 @@
         <v>25</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:28" ht="12.75">
@@ -2145,10 +2145,10 @@
         <v>7</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="36" t="s">
@@ -2181,10 +2181,10 @@
         <v>25</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E39" s="29"/>
       <c r="F39" s="30"/>
@@ -2197,10 +2197,10 @@
         <v>25</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="27"/>
@@ -2213,10 +2213,10 @@
         <v>7</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" s="35"/>
       <c r="F41" s="36" t="s">
@@ -2231,10 +2231,10 @@
         <v>25</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="27"/>
@@ -2247,10 +2247,10 @@
         <v>25</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="27"/>
@@ -2263,10 +2263,10 @@
         <v>25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="27"/>
@@ -2279,14 +2279,14 @@
         <v>25</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45" s="45"/>
       <c r="F45" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="13.5" thickBot="1">
@@ -2297,10 +2297,10 @@
         <v>7</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" s="47"/>
       <c r="F46" s="41" t="s">
@@ -2309,68 +2309,68 @@
     </row>
     <row r="47" spans="1:28" ht="12.75">
       <c r="A47" s="66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E47" s="48"/>
       <c r="F47" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="12.75">
+      <c r="A48" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="49" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" ht="12.75">
-      <c r="A48" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="49" t="s">
+      <c r="C48" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="D48" s="25" t="s">
         <v>90</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="E48" s="29"/>
       <c r="F48" s="31"/>
     </row>
     <row r="49" spans="1:16384" ht="12.75">
       <c r="A49" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:16384" ht="12.75">
       <c r="A50" s="68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="50" t="s">
@@ -2379,54 +2379,54 @@
     </row>
     <row r="51" spans="1:16384" ht="12.75">
       <c r="A51" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C51" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="26" t="s">
+      <c r="F51" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="51" t="s">
+    </row>
+    <row r="52" spans="1:16384" ht="12.75">
+      <c r="A52" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:16384" ht="12.75">
-      <c r="A52" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>99</v>
-      </c>
       <c r="D52" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:16384" ht="12.75">
       <c r="A53" s="68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E53" s="35"/>
       <c r="F53" s="50" t="s">
@@ -2435,68 +2435,68 @@
     </row>
     <row r="54" spans="1:16384" ht="12.75">
       <c r="A54" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B54" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E54" s="29"/>
       <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:16384" ht="12.75">
       <c r="A55" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D55" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="26" t="s">
+      <c r="F55" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="F55" s="27" t="s">
+    </row>
+    <row r="56" spans="1:16384" ht="12.75">
+      <c r="A56" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:16384" ht="12.75">
-      <c r="A56" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="24" t="s">
+      <c r="D56" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>109</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="27"/>
     </row>
     <row r="57" spans="1:16384" ht="12.75">
       <c r="A57" s="68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E57" s="35"/>
       <c r="F57" s="36" t="s">
@@ -2505,118 +2505,118 @@
     </row>
     <row r="58" spans="1:16384" ht="12.75">
       <c r="A58" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="25" t="s">
+      <c r="E58" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="E58" s="26" t="s">
+      <c r="F58" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="27" t="s">
+    </row>
+    <row r="59" spans="1:16384" ht="12.75">
+      <c r="A59" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="24" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:16384" ht="12.75">
-      <c r="A59" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>116</v>
-      </c>
       <c r="D59" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="27"/>
     </row>
     <row r="60" spans="1:16384" ht="12.75">
       <c r="A60" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D60" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="27"/>
     </row>
     <row r="61" spans="1:16384" s="1" customFormat="1" ht="12.75">
       <c r="A61" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="27"/>
     </row>
     <row r="62" spans="1:16384" ht="13.5" thickBot="1">
       <c r="A62" s="69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E62" s="52"/>
       <c r="F62" s="41"/>
     </row>
     <row r="63" spans="1:16384" ht="13.5" thickBot="1">
       <c r="A63" s="70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E63" s="94"/>
       <c r="F63" s="95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:16384" s="10" customFormat="1" ht="12.75">
       <c r="A64" s="79" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B64" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D64" s="81" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E64" s="85"/>
       <c r="F64" s="86"/>
@@ -19001,16 +19001,16 @@
     </row>
     <row r="65" spans="1:16384" s="10" customFormat="1" ht="13.5" thickBot="1">
       <c r="A65" s="82" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B65" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="83" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D65" s="84" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E65" s="90"/>
       <c r="F65" s="91"/>
@@ -35396,7 +35396,7 @@
     <row r="66" spans="1:16384" ht="12.75">
       <c r="A66" s="11"/>
       <c r="B66" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="14"/>
@@ -35405,130 +35405,130 @@
     <row r="67" spans="1:16384" ht="12.75">
       <c r="A67" s="11"/>
       <c r="B67" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C67" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D67" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F67" s="13"/>
     </row>
     <row r="68" spans="1:16384" ht="12.75">
       <c r="A68" s="16"/>
       <c r="B68" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D68" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:16384" ht="12.75">
       <c r="A69" s="16"/>
       <c r="B69" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C69" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D69" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:16384" ht="12.75">
       <c r="A70" s="11"/>
       <c r="B70" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="D70" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:16384" ht="12.75">
       <c r="A71" s="11"/>
       <c r="B71" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D71" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F71" s="13"/>
     </row>
     <row r="72" spans="1:16384" ht="12.75">
       <c r="A72" s="11"/>
       <c r="B72" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C72" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D72" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F72" s="13"/>
     </row>
     <row r="73" spans="1:16384" ht="12.75">
       <c r="A73" s="11"/>
       <c r="B73" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C73" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="D73" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F73" s="13"/>
     </row>
     <row r="74" spans="1:16384" ht="12.75">
       <c r="A74" s="11"/>
       <c r="B74" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F74" s="13"/>
     </row>
     <row r="75" spans="1:16384" ht="12.75">
       <c r="A75" s="11"/>
       <c r="B75" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F75" s="13"/>
     </row>
     <row r="76" spans="1:16384" ht="12.75">
       <c r="A76" s="11"/>
       <c r="B76" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F76" s="13"/>
     </row>

</xml_diff>

<commit_message>
* Turns out if I don't set buttons to non interactable at the start of the tutorial, even if they're not visible, the hotkeys will still work, so they need to be set as non interactable and not in an interactable game stage right from the start for the tutorial. * Dialogue adjustments. * Moving the dialogue boxes back in front of the terraforming and store disperse UIs
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DA294A2A-F58E-42DC-BF37-2E844AB11A08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9086F74-7DBB-4C2C-AF47-3BAF1E2D88DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,25 +403,7 @@
     <t>Juice: Typewriter FX</t>
   </si>
   <si>
-    <t>Task: build an /ice drill\.</t>
-  </si>
-  <si>
-    <t>Task: build a @gas pump$.</t>
-  </si>
-  <si>
-    <t>Task: build a /boiler\.</t>
-  </si>
-  <si>
-    <t>Task: build a [fusion reactor].</t>
-  </si>
-  <si>
     <t>Task: gather 4 +minerals&amp;.</t>
-  </si>
-  <si>
-    <t>Task: build a &lt;turret&gt;.</t>
-  </si>
-  <si>
-    <t>Build turrets to defend your base.</t>
   </si>
   <si>
     <t>Detected +minerals&amp;.</t>
@@ -490,9 +472,6 @@
     <t>That's all you need to know. Good luck out there soldier! Don't die!</t>
   </si>
   <si>
-    <t>You can see your overall terraforming progress here. Press P to disable this menu again.</t>
-  </si>
-  <si>
     <t>This planet is currently inadequate for human life, fortunately you have been equipped with me!</t>
   </si>
   <si>
@@ -503,9 +482,6 @@
   </si>
   <si>
     <t>Awesome. Now that you've got power, you'll need these buildings to collect resources for your base.</t>
-  </si>
-  <si>
-    <t>Because you have enough /water\ and @gas$, I'll get you to build a /boiler\ first.</t>
   </si>
   <si>
     <t>If you need less of one of your terraforming buildings, clicking on it will give you options for disabling or demolishing it. Try it.</t>
@@ -523,16 +499,10 @@
     <t>To retrieve a dialogue set in-code, you need to retrieve it with the exact value listed in the Dialogue Key column.</t>
   </si>
   <si>
-    <t>Now, build a @gas pump$! Look for a green patch.</t>
-  </si>
-  <si>
     <t>Keep in mind that you'll need to build on areas with the appropriate resources.</t>
   </si>
   <si>
     <t>Stored in my memory are blueprints of buildings that can be used to make this barren planet a paradise for your humans.</t>
-  </si>
-  <si>
-    <t>First, you'll need power. Please build a [fusion reactor].</t>
   </si>
   <si>
     <t>Skipped Tutorial</t>
@@ -551,9 +521,6 @@
   </si>
   <si>
     <t>got resources</t>
-  </si>
-  <si>
-    <t>Try building an /ice drill\! Look for a blue patch.</t>
   </si>
   <si>
     <t>The gold sections show your target building counts! Try to build as close to this as you can.</t>
@@ -584,6 +551,39 @@
   </si>
   <si>
     <t>D.O.G. OUT! U^w^U</t>
+  </si>
+  <si>
+    <t>Task: build a [Fusion Reactor].</t>
+  </si>
+  <si>
+    <t>First, you'll need power. Please build a [Fusion Reactor].</t>
+  </si>
+  <si>
+    <t>Task: build an /Ice Drill\.</t>
+  </si>
+  <si>
+    <t>Task: build a @Gas Pump$.</t>
+  </si>
+  <si>
+    <t>Now, build a @Gas Pump$! Look for a yellowy-green patch.</t>
+  </si>
+  <si>
+    <t>Task: build a /Boiler\.</t>
+  </si>
+  <si>
+    <t>Because you have enough /water\ and @gas$, I'll get you to build a /Boiler\ first.</t>
+  </si>
+  <si>
+    <t>You can see your overall terraforming progress here. Press P again to disable this menu again.</t>
+  </si>
+  <si>
+    <t>Task: build a &lt;Turret&gt;.</t>
+  </si>
+  <si>
+    <t>Build &lt;Turrets&gt; to defend your base.</t>
+  </si>
+  <si>
+    <t>Try building an /Ice Drill\! Look for a blue patch. If you need more minerals, go and do some mining first.</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
   <dimension ref="A1:XFD995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1405,16 +1405,16 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="12.75">
       <c r="A2" s="56" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="27"/>
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
@@ -1496,13 +1496,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
@@ -1512,13 +1512,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -1528,13 +1528,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="30"/>
@@ -1550,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27" t="s">
@@ -1586,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
@@ -1602,7 +1602,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -1618,7 +1618,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
@@ -1634,7 +1634,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1650,7 +1650,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="31"/>
@@ -1684,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="27" t="s">
@@ -1702,7 +1702,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
@@ -1718,7 +1718,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="36" t="s">
@@ -1758,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>36</v>
@@ -1778,7 +1778,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="41" t="s">
@@ -1812,7 +1812,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="71" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27" t="s">
@@ -1852,7 +1852,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36" t="s">
@@ -1892,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="71" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>47</v>
@@ -1912,7 +1912,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -1930,7 +1930,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
@@ -1946,7 +1946,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="36" t="s">
@@ -1986,7 +1986,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>53</v>
@@ -2006,7 +2006,7 @@
         <v>55</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="36" t="s">
@@ -2024,7 +2024,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="72" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>57</v>
@@ -2041,7 +2041,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>60</v>
@@ -2062,7 +2062,7 @@
         <v>62</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="36" t="s">
@@ -2102,7 +2102,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="27" t="s">
@@ -2138,7 +2138,7 @@
         <v>65</v>
       </c>
       <c r="D37" s="71" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="27" t="s">
@@ -2208,7 +2208,7 @@
         <v>73</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="27"/>
@@ -2242,7 +2242,7 @@
         <v>76</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="27"/>
@@ -2258,7 +2258,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="27"/>
@@ -2274,7 +2274,7 @@
         <v>78</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="27"/>
@@ -2290,7 +2290,7 @@
         <v>78</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E45" s="45"/>
       <c r="F45" s="27" t="s">
@@ -2378,7 +2378,7 @@
         <v>92</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="50" t="s">
@@ -2396,7 +2396,7 @@
         <v>93</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>132</v>
+        <v>185</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>94</v>
@@ -2416,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="51" t="s">
@@ -2434,7 +2434,7 @@
         <v>98</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E53" s="35"/>
       <c r="F53" s="50" t="s">
@@ -2488,7 +2488,7 @@
         <v>104</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E56" s="35"/>
       <c r="F56" s="36" t="s">
@@ -2501,10 +2501,10 @@
         <v>86</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D57" s="98" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E57" s="99"/>
       <c r="F57" s="100"/>
@@ -2520,7 +2520,7 @@
         <v>105</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E58" s="26" t="s">
         <v>106</v>
@@ -2540,7 +2540,7 @@
         <v>108</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="27"/>
@@ -2554,7 +2554,7 @@
         <v>108</v>
       </c>
       <c r="D60" s="98" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="27"/>
@@ -2568,7 +2568,7 @@
         <v>108</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="27"/>
@@ -2584,7 +2584,7 @@
         <v>78</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="27"/>
@@ -2600,7 +2600,7 @@
         <v>78</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E63" s="29"/>
       <c r="F63" s="27"/>
@@ -2641,16 +2641,16 @@
     </row>
     <row r="66" spans="1:16384" s="10" customFormat="1" ht="12.75">
       <c r="A66" s="79" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B66" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="80" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D66" s="81" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E66" s="85"/>
       <c r="F66" s="86"/>
@@ -19035,16 +19035,16 @@
     </row>
     <row r="67" spans="1:16384" s="10" customFormat="1" ht="13.5" thickBot="1">
       <c r="A67" s="82" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B67" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="83" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D67" s="84" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E67" s="90"/>
       <c r="F67" s="91"/>
@@ -35445,7 +35445,7 @@
         <v>116</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F69" s="13"/>
     </row>
@@ -35458,7 +35458,7 @@
         <v>116</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F70" s="13"/>
     </row>
@@ -35471,7 +35471,7 @@
         <v>116</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F71" s="13"/>
     </row>

</xml_diff>

<commit_message>
UPDATE: Tutorial dialogue, minor fix to tag/layer
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgkha\Desktop\Capstone 2020\P.O.D\Unity Project\2020GP-Cap-Stone-2020\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9086F74-7DBB-4C2C-AF47-3BAF1E2D88DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A6FC35-E2B6-4324-85C1-3686706DAB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue, v2.xlsx" sheetId="1" r:id="rId1"/>
@@ -403,9 +403,6 @@
     <t>Juice: Typewriter FX</t>
   </si>
   <si>
-    <t>Task: gather 4 +minerals&amp;.</t>
-  </si>
-  <si>
     <t>Detected +minerals&amp;.</t>
   </si>
   <si>
@@ -476,9 +473,6 @@
   </si>
   <si>
     <t>Firstly, we are going to need some building materials.</t>
-  </si>
-  <si>
-    <t>Please gather 4 +minerals&amp;.</t>
   </si>
   <si>
     <t>Awesome. Now that you've got power, you'll need these buildings to collect resources for your base.</t>
@@ -584,6 +578,12 @@
   </si>
   <si>
     <t>Try building an /Ice Drill\! Look for a blue patch. If you need more minerals, go and do some mining first.</t>
+  </si>
+  <si>
+    <t>Please gather 3 +minerals&amp;.</t>
+  </si>
+  <si>
+    <t>Task: gather 3 +minerals&amp;.</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1370,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1405,16 +1405,16 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="12.75">
       <c r="A2" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="27"/>
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
@@ -1496,13 +1496,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
@@ -1512,13 +1512,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -1528,13 +1528,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="30"/>
@@ -1550,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27" t="s">
@@ -1586,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
@@ -1602,7 +1602,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -1618,7 +1618,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
@@ -1634,7 +1634,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1650,7 +1650,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="31"/>
@@ -1684,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="27" t="s">
@@ -1702,7 +1702,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
@@ -1718,7 +1718,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="36" t="s">
@@ -1758,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>36</v>
@@ -1778,7 +1778,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="41" t="s">
@@ -1812,7 +1812,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27" t="s">
@@ -1852,7 +1852,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36" t="s">
@@ -1892,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="71" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>47</v>
@@ -1912,7 +1912,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -1930,7 +1930,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
@@ -1946,7 +1946,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="36" t="s">
@@ -1986,7 +1986,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>53</v>
@@ -2006,7 +2006,7 @@
         <v>55</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="36" t="s">
@@ -2024,7 +2024,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>57</v>
@@ -2041,7 +2041,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>60</v>
@@ -2062,7 +2062,7 @@
         <v>62</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="36" t="s">
@@ -2102,7 +2102,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="27" t="s">
@@ -2138,7 +2138,7 @@
         <v>65</v>
       </c>
       <c r="D37" s="71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="27" t="s">
@@ -2208,7 +2208,7 @@
         <v>73</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="27"/>
@@ -2242,7 +2242,7 @@
         <v>76</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="27"/>
@@ -2258,7 +2258,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="27"/>
@@ -2274,7 +2274,7 @@
         <v>78</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="27"/>
@@ -2290,7 +2290,7 @@
         <v>78</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" s="45"/>
       <c r="F45" s="27" t="s">
@@ -2378,7 +2378,7 @@
         <v>92</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="50" t="s">
@@ -2396,7 +2396,7 @@
         <v>93</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>94</v>
@@ -2416,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="51" t="s">
@@ -2434,7 +2434,7 @@
         <v>98</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E53" s="35"/>
       <c r="F53" s="50" t="s">
@@ -2488,7 +2488,7 @@
         <v>104</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="35"/>
       <c r="F56" s="36" t="s">
@@ -2501,10 +2501,10 @@
         <v>86</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D57" s="98" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E57" s="99"/>
       <c r="F57" s="100"/>
@@ -2520,7 +2520,7 @@
         <v>105</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E58" s="26" t="s">
         <v>106</v>
@@ -2540,7 +2540,7 @@
         <v>108</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="27"/>
@@ -2554,7 +2554,7 @@
         <v>108</v>
       </c>
       <c r="D60" s="98" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="27"/>
@@ -2568,7 +2568,7 @@
         <v>108</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="27"/>
@@ -2584,7 +2584,7 @@
         <v>78</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="27"/>
@@ -2600,7 +2600,7 @@
         <v>78</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E63" s="29"/>
       <c r="F63" s="27"/>
@@ -2641,16 +2641,16 @@
     </row>
     <row r="66" spans="1:16384" s="10" customFormat="1" ht="12.75">
       <c r="A66" s="79" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B66" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D66" s="81" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E66" s="85"/>
       <c r="F66" s="86"/>
@@ -19035,16 +19035,16 @@
     </row>
     <row r="67" spans="1:16384" s="10" customFormat="1" ht="13.5" thickBot="1">
       <c r="A67" s="82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B67" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="83" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D67" s="84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E67" s="90"/>
       <c r="F67" s="91"/>
@@ -35445,7 +35445,7 @@
         <v>116</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F69" s="13"/>
     </row>
@@ -35458,7 +35458,7 @@
         <v>116</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F70" s="13"/>
     </row>
@@ -35471,7 +35471,7 @@
         <v>116</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F71" s="13"/>
     </row>

</xml_diff>

<commit_message>
FIX: Combat stage to wait til all initial aliens are killed before moving on to next dialogue
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue, v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgkha\Desktop\Capstone 2020\P.O.D\Unity Project\2020GP-Cap-Stone-2020\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A6FC35-E2B6-4324-85C1-3686706DAB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1ADEB6-FED5-4691-8BB6-A80B415543A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,9 +325,6 @@
     <t>shoot</t>
   </si>
   <si>
-    <t>You also have an on-board laser cannon to defend yourself with.</t>
-  </si>
-  <si>
     <t>Press space to shoot.</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>heal at cryo egg</t>
   </si>
   <si>
-    <t>Weapon systems online.~Task: shoot with your on-board laser cannon by pressing the spacebar.</t>
-  </si>
-  <si>
     <t>Task: heal yourself at the terraforming tower by holding E.</t>
   </si>
   <si>
@@ -584,6 +578,12 @@
   </si>
   <si>
     <t>Task: gather 3 +minerals&amp;.</t>
+  </si>
+  <si>
+    <t>You also have an on-board laser cannon to defend yourself with. If you've got any aliens left, clear them all out!</t>
+  </si>
+  <si>
+    <t>Weapon systems online.~Task: shoot with your on-board laser cannon by pressing the spacebar. If you've got any aliens left, clear them all out.</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
   <dimension ref="A1:XFD995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1405,16 +1405,16 @@
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="12.75">
       <c r="A2" s="56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="27"/>
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
@@ -1496,13 +1496,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
@@ -1512,13 +1512,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -1528,13 +1528,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="30"/>
@@ -1550,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27" t="s">
@@ -1586,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
@@ -1602,7 +1602,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
@@ -1618,7 +1618,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
@@ -1634,7 +1634,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
@@ -1650,7 +1650,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="31"/>
@@ -1684,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="27" t="s">
@@ -1702,7 +1702,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
@@ -1718,7 +1718,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="36" t="s">
@@ -1758,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>36</v>
@@ -1778,7 +1778,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="41" t="s">
@@ -1812,7 +1812,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="71" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27" t="s">
@@ -1852,7 +1852,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E25" s="35"/>
       <c r="F25" s="36" t="s">
@@ -1892,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>47</v>
@@ -1912,7 +1912,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
@@ -1930,7 +1930,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="73" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
@@ -1946,7 +1946,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="36" t="s">
@@ -1986,7 +1986,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="71" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>53</v>
@@ -2006,7 +2006,7 @@
         <v>55</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="36" t="s">
@@ -2024,7 +2024,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="72" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E32" s="40" t="s">
         <v>57</v>
@@ -2041,7 +2041,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>60</v>
@@ -2062,7 +2062,7 @@
         <v>62</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="36" t="s">
@@ -2102,7 +2102,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="27" t="s">
@@ -2138,7 +2138,7 @@
         <v>65</v>
       </c>
       <c r="D37" s="71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="27" t="s">
@@ -2208,7 +2208,7 @@
         <v>73</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="27"/>
@@ -2242,7 +2242,7 @@
         <v>76</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="27"/>
@@ -2258,7 +2258,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="27"/>
@@ -2274,7 +2274,7 @@
         <v>78</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="27"/>
@@ -2290,7 +2290,7 @@
         <v>78</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45" s="45"/>
       <c r="F45" s="27" t="s">
@@ -2378,7 +2378,7 @@
         <v>92</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E50" s="35"/>
       <c r="F50" s="50" t="s">
@@ -2396,7 +2396,7 @@
         <v>93</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>94</v>
@@ -2416,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="51" t="s">
@@ -2434,7 +2434,7 @@
         <v>98</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="E53" s="35"/>
       <c r="F53" s="50" t="s">
@@ -2452,7 +2452,7 @@
         <v>99</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="E54" s="29"/>
       <c r="F54" s="30"/>
@@ -2468,13 +2468,13 @@
         <v>99</v>
       </c>
       <c r="D55" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E55" s="26" t="s">
+      <c r="F55" s="27" t="s">
         <v>102</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75">
@@ -2485,10 +2485,10 @@
         <v>7</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E56" s="35"/>
       <c r="F56" s="36" t="s">
@@ -2501,10 +2501,10 @@
         <v>86</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D57" s="98" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E57" s="99"/>
       <c r="F57" s="100"/>
@@ -2517,16 +2517,16 @@
         <v>14</v>
       </c>
       <c r="C58" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="D58" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="26" t="s">
+      <c r="F58" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="F58" s="27" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75">
@@ -2537,10 +2537,10 @@
         <v>86</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="27"/>
@@ -2551,10 +2551,10 @@
         <v>86</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D60" s="98" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="27"/>
@@ -2565,10 +2565,10 @@
         <v>86</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="27"/>
@@ -2584,7 +2584,7 @@
         <v>78</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="27"/>
@@ -2600,7 +2600,7 @@
         <v>78</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E63" s="29"/>
       <c r="F63" s="27"/>
@@ -2613,44 +2613,44 @@
         <v>7</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D64" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E64" s="52"/>
       <c r="F64" s="41"/>
     </row>
     <row r="65" spans="1:16384" ht="13.5" thickBot="1">
       <c r="A65" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E65" s="94"/>
       <c r="F65" s="95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:16384" s="10" customFormat="1" ht="12.75">
       <c r="A66" s="79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B66" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D66" s="81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E66" s="85"/>
       <c r="F66" s="86"/>
@@ -19035,16 +19035,16 @@
     </row>
     <row r="67" spans="1:16384" s="10" customFormat="1" ht="13.5" thickBot="1">
       <c r="A67" s="82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D67" s="84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E67" s="90"/>
       <c r="F67" s="91"/>
@@ -35430,7 +35430,7 @@
     <row r="68" spans="1:16384" ht="12.75">
       <c r="A68" s="11"/>
       <c r="B68" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="14"/>
@@ -35439,130 +35439,130 @@
     <row r="69" spans="1:16384" ht="12.75">
       <c r="A69" s="11"/>
       <c r="B69" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D69" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:16384" ht="12.75">
       <c r="A70" s="16"/>
       <c r="B70" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C70" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D70" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:16384" ht="12.75">
       <c r="A71" s="16"/>
       <c r="B71" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D71" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F71" s="13"/>
     </row>
     <row r="72" spans="1:16384" ht="12.75">
       <c r="A72" s="11"/>
       <c r="B72" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="D72" s="14" t="s">
         <v>116</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>117</v>
       </c>
       <c r="F72" s="13"/>
     </row>
     <row r="73" spans="1:16384" ht="12.75">
       <c r="A73" s="11"/>
       <c r="B73" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C73" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D73" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F73" s="13"/>
     </row>
     <row r="74" spans="1:16384" ht="12.75">
       <c r="A74" s="11"/>
       <c r="B74" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D74" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F74" s="13"/>
     </row>
     <row r="75" spans="1:16384" ht="12.75">
       <c r="A75" s="11"/>
       <c r="B75" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C75" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C75" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="D75" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F75" s="13"/>
     </row>
     <row r="76" spans="1:16384" ht="12.75">
       <c r="A76" s="11"/>
       <c r="B76" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F76" s="13"/>
     </row>
     <row r="77" spans="1:16384" ht="12.75">
       <c r="A77" s="11"/>
       <c r="B77" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F77" s="13"/>
     </row>
     <row r="78" spans="1:16384" ht="12.75">
       <c r="A78" s="11"/>
       <c r="B78" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F78" s="13"/>
     </row>

</xml_diff>